<commit_message>
Added 2 more quarters
</commit_message>
<xml_diff>
--- a/Test docs/Test Excel file.xlsx
+++ b/Test docs/Test Excel file.xlsx
@@ -16,12 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Q1</t>
   </si>
   <si>
     <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
   </si>
 </sst>
 </file>
@@ -360,20 +366,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made a new flag
</commit_message>
<xml_diff>
--- a/Test docs/Test Excel file.xlsx
+++ b/Test docs/Test Excel file.xlsx
@@ -43,12 +43,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -63,8 +87,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,8 +416,117 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Reverted to version 4
</commit_message>
<xml_diff>
--- a/Test docs/Test Excel file.xlsx
+++ b/Test docs/Test Excel file.xlsx
@@ -16,18 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Q1</t>
   </si>
   <si>
     <t>Q2</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>Q4</t>
   </si>
 </sst>
 </file>
@@ -43,36 +37,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF002060"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -87,12 +57,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,139 +360,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>